<commit_message>
Add todo list, change feature list.
</commit_message>
<xml_diff>
--- a/FeatureList.xlsx
+++ b/FeatureList.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DCF6741D-EBED-45FB-90A9-35B33694647F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{70872D39-C13C-4A40-AD49-FD8ADF849389}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$57</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -733,10 +736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1116,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1130,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
@@ -1332,7 +1336,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
@@ -1416,7 +1420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
@@ -1430,10 +1434,10 @@
         <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
@@ -1458,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
@@ -1469,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -1486,10 +1490,10 @@
         <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
@@ -1503,10 +1507,10 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -1567,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -1578,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -1601,6 +1605,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F57" xr:uid="{60200546-B511-4D01-8607-1D4A6F83BC5C}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="0.1.0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F41:F44 F35:F36 E2:F2 E3:E57 F3:F20">
     <cfRule type="colorScale" priority="3">

</xml_diff>

<commit_message>
Create UML and scenario descriptions file. Update readme.txt to readme.md Update TODO list
</commit_message>
<xml_diff>
--- a/FeatureList.xlsx
+++ b/FeatureList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{70872D39-C13C-4A40-AD49-FD8ADF849389}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{536EBDE5-5CCD-48A4-9588-691E779745DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="91">
   <si>
     <t>M</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +130,6 @@
   </si>
   <si>
     <t>显示匹配结果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -739,8 +735,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -751,33 +747,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -794,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -811,7 +807,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -825,10 +821,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -845,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -862,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -876,10 +872,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -896,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -913,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -930,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -947,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -964,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -981,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -998,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -1012,10 +1008,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
@@ -1032,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -1049,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -1066,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
@@ -1083,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -1100,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
         <v>0</v>
@@ -1114,7 +1110,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1128,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1142,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
@@ -1156,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1170,10 +1166,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1184,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1195,7 +1191,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1206,24 +1202,24 @@
         <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
         <v>0</v>
@@ -1237,10 +1233,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
@@ -1251,10 +1247,10 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
@@ -1268,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
         <v>0</v>
@@ -1282,7 +1278,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
         <v>0</v>
@@ -1293,36 +1289,36 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E35" t="s">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1330,10 +1326,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1341,10 +1337,10 @@
         <v>2</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1352,10 +1348,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1363,10 +1359,10 @@
         <v>2</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1374,10 +1370,10 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
@@ -1391,10 +1387,10 @@
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" t="s">
         <v>14</v>
@@ -1407,9 +1403,6 @@
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
-        <v>27</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>26</v>
       </c>
@@ -1434,7 +1427,7 @@
         <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1490,7 +1483,7 @@
         <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1507,7 +1500,7 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>